<commit_message>
added procedure - full reload data from Landing to Stg1, added usp_write_log for logging procedures that were run
</commit_message>
<xml_diff>
--- a/mapping_docs/cars-com_card mapping.xlsx
+++ b/mapping_docs/cars-com_card mapping.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="180">
   <si>
     <t>Data Example lnd_cars-com_card</t>
   </si>
@@ -224,7 +224,7 @@
     <t>example (based on example 1st sheet) of source data</t>
   </si>
   <si>
-    <t>IDENTITY, PK</t>
+    <t>PK</t>
   </si>
   <si>
     <r>
@@ -254,42 +254,17 @@
     <t>row_id</t>
   </si>
   <si>
-    <t>INT</t>
+    <t>UUID</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>CURRENT_TIMESTAMP</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>2023-04-29 01:19:40.000</t>
-  </si>
-  <si>
-    <t>BK</t>
-  </si>
-  <si>
-    <t>VARCHAR(100)</t>
-  </si>
-  <si>
-    <t>direct</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>`paid-project-346208`</t>
+    <t>38237b95-2195-47ae-8d73-9c6e344c7b2c</t>
+  </si>
+  <si>
+    <r>
+      <t>GENERATE_UUID</t>
     </r>
     <r>
       <rPr>
@@ -298,7 +273,28 @@
         <rFont val="Consolas"/>
         <charset val="204"/>
       </rPr>
-      <t>.</t>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>direct</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>`paid-project-346208`</t>
     </r>
     <r>
       <rPr>
@@ -307,6 +303,15 @@
         <rFont val="Consolas"/>
         <charset val="204"/>
       </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="204"/>
+      </rPr>
       <t>car_ads_ds_landing</t>
     </r>
   </si>
@@ -388,7 +393,10 @@
     </r>
   </si>
   <si>
-    <t>VARCHAR(MAX)</t>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>stg_car_card_prices or json</t>
@@ -397,9 +405,6 @@
     <t>adress</t>
   </si>
   <si>
-    <t>VARCHAR(200)</t>
-  </si>
-  <si>
     <t>60 S Broadway Salem</t>
   </si>
   <si>
@@ -432,9 +437,6 @@
     <t>state</t>
   </si>
   <si>
-    <t>VARCHAR(50)</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
@@ -551,6 +553,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Great Deal | $1,086 under|</t>
     </r>
     <r>
@@ -583,6 +592,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Great Deal | $1,086 under|Home Delivery|</t>
     </r>
     <r>
@@ -650,6 +666,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">2022, 6-Speed </t>
     </r>
     <r>
@@ -720,6 +743,9 @@
     <t>engine</t>
   </si>
   <si>
+    <t>NUMERIC</t>
+  </si>
+  <si>
     <t>split by pipeline, take the first value and then split by comma, take the third value. Find value as  X.XL format with splitting by space. The result transform from X.XL to XX00 format (example: 2.0L -&gt; 2000)</t>
   </si>
   <si>
@@ -763,6 +789,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">2022, 6-Speed Automatic, 2.0L </t>
     </r>
     <r>
@@ -843,6 +876,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>2022, 6-Speed Automatic, 2.0L I4 16V GDI DOHC, Gasoline (</t>
     </r>
     <r>
@@ -917,6 +957,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">2022, 6-Speed Automatic, 2.0L I4 16V GDI DOHC, Gasoline (23–29 mpg), 3.395 </t>
     </r>
     <r>
@@ -1056,6 +1103,82 @@
       </rPr>
       <t>Ruby Red</t>
     </r>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>input_file_name</t>
+  </si>
+  <si>
+    <t>file:/C:/Users/gavri/PycharmProjects/car_ads_scrapper/scrapped_data/cars_com/json/2023-05-14-05-42-14/2021/price_50000-59999/https---www-cars-com-vehicledetail-58ea2312-4dac-416b-a479-7d068d02b03a-.json</t>
+  </si>
+  <si>
+    <t>dl_loaded_date</t>
+  </si>
+  <si>
+    <t>2023-04-20 10:21:56.576</t>
+  </si>
+  <si>
+    <t>2023-05-16 10:21:56.576</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>stg1_loaded_date</t>
+  </si>
+  <si>
+    <t>2023-04-29 01:19:40.000</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP()</t>
+  </si>
+  <si>
+    <t>SHA256()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>`paid-project-346209`</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <charset val="204"/>
+      </rPr>
+      <t>.car_ads_ds_landing</t>
+    </r>
+  </si>
+  <si>
+    <t>row_hash</t>
+  </si>
+  <si>
+    <t>BYTES(32)</t>
+  </si>
+  <si>
+    <t>,â átg¯gí  0 «# [ Z¯¹tùÎBñÿ¼=  Ü</t>
+  </si>
+  <si>
+    <t>SHA256(CONCAT(
+   IFNULL(card_id, ''),
+   IFNULL(title, ''),
+   IFNULL(price_primary, ''),
+   IFNULL(price_history, ''),
+   IFNULL(location, ''),
+   IFNULL(labels, ''),
+   IFNULL(comment, ''),
+   IFNULL(description, ''),
+   IFNULL(vehicle_history, '')
+   ))</t>
   </si>
 </sst>
 </file>
@@ -1064,9 +1187,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1126,12 +1249,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1139,6 +1263,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1153,22 +1285,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1192,30 +1316,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1229,15 +1330,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1266,13 +1375,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1311,12 +1434,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1329,25 +1446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,19 +1464,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1389,49 +1488,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,31 +1506,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1492,6 +1579,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1872,150 +1989,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2050,23 +2167,17 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2076,12 +2187,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2106,11 +2220,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2119,19 +2233,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2140,10 +2254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2151,7 +2265,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2876,238 +2990,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:4">
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:1">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="15.75" spans="1:10">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="51" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <v>212900</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="52" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>82996</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="29"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="35">
+      <c r="A6" s="34">
         <v>23070</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>29997</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="53" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36">
         <v>45669</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:10">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="39">
         <v>25795</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="54" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" ht="15.75"/>
     <row r="11" spans="1:4">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="47"/>
+      <c r="D12" s="46"/>
     </row>
     <row r="13" ht="15.75" spans="1:4">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="38" t="s">
+      <c r="B13" s="48"/>
+      <c r="C13" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="50"/>
+      <c r="D13" s="49"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="51"/>
+      <c r="B15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3129,10 +3243,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N33"/>
+  <dimension ref="A3:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3214,7 +3328,7 @@
       <c r="M4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="14"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:14">
       <c r="A5" s="4" t="s">
@@ -3236,19 +3350,21 @@
         <v>74</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15"/>
+      <c r="H5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="14"/>
+      <c r="N5" s="11"/>
     </row>
-    <row r="6" customFormat="1" spans="1:14">
+    <row r="6" spans="1:14">
       <c r="A6" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>70</v>
@@ -3257,29 +3373,37 @@
         <v>71</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>70</v>
       </c>
@@ -3287,36 +3411,36 @@
         <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="19"/>
+      <c r="L7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" ht="25.5" spans="1:14">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>70</v>
@@ -3325,36 +3449,36 @@
         <v>71</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L8" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="N8" s="19"/>
+      <c r="M8" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" s="18"/>
     </row>
-    <row r="9" ht="25.5" spans="1:14">
+    <row r="9" spans="1:14">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>70</v>
@@ -3363,34 +3487,34 @@
         <v>71</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="N9" s="19"/>
+      <c r="H9" s="5">
+        <v>25795</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="17">
+        <v>25795</v>
+      </c>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="6"/>
@@ -3401,34 +3525,36 @@
         <v>71</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="5">
-        <v>25795</v>
-      </c>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" s="18">
-        <v>25795</v>
-      </c>
-      <c r="N10" s="19"/>
+      <c r="L10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="6"/>
@@ -3439,38 +3565,36 @@
         <v>71</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>93</v>
-      </c>
+      <c r="L11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" ht="25.5" spans="1:14">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
         <v>70</v>
@@ -3479,36 +3603,36 @@
         <v>71</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="N12" s="19"/>
+      <c r="M12" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="N12" s="18"/>
     </row>
-    <row r="13" ht="25.5" spans="1:14">
+    <row r="13" ht="38.25" spans="1:14">
       <c r="A13" s="6"/>
       <c r="B13" s="4" t="s">
         <v>70</v>
@@ -3517,34 +3641,34 @@
         <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="5">
+        <v>3079</v>
+      </c>
+      <c r="I13" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" s="17" t="s">
+      <c r="J13" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="19"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" ht="38.25" spans="1:14">
       <c r="A14" s="6"/>
@@ -3558,33 +3682,33 @@
         <v>104</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5">
-        <v>3079</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="N14" s="19"/>
+      <c r="K14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N14" s="18"/>
     </row>
-    <row r="15" ht="38.25" spans="1:14">
+    <row r="15" ht="25.5" spans="1:14">
       <c r="A15" s="6"/>
       <c r="B15" s="4" t="s">
         <v>70</v>
@@ -3593,34 +3717,36 @@
         <v>71</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="H15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="N15" s="19"/>
+      <c r="M15" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" ht="25.5" spans="1:14">
       <c r="A16" s="6"/>
@@ -3631,98 +3757,96 @@
         <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" s="17" t="s">
+      <c r="J16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="N16" s="19"/>
+      <c r="N16" s="18"/>
     </row>
-    <row r="17" ht="25.5" spans="1:14">
+    <row r="17" spans="1:14">
       <c r="A17" s="6"/>
-      <c r="B17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="N17" s="19"/>
+      <c r="N17" s="18"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="6"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="M18" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="N18" s="19"/>
+      <c r="H18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" ht="25.5" spans="1:14">
       <c r="A19" s="6"/>
       <c r="B19" s="4" t="s">
         <v>70</v>
@@ -3731,36 +3855,36 @@
         <v>71</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I19" s="20" t="s">
+      <c r="H19" s="5">
+        <v>2022</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="19"/>
+      <c r="L19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="N19" s="18"/>
     </row>
-    <row r="20" ht="25.5" spans="1:14">
+    <row r="20" ht="51" spans="1:14">
       <c r="A20" s="6"/>
       <c r="B20" s="4" t="s">
         <v>70</v>
@@ -3772,33 +3896,33 @@
         <v>121</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="5">
-        <v>2022</v>
-      </c>
-      <c r="I20" s="20" t="s">
+      <c r="H20" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L20" s="17" t="s">
+      <c r="I20" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="N20" s="19"/>
+      <c r="M20" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" s="18"/>
     </row>
-    <row r="21" ht="51" spans="1:14">
+    <row r="21" ht="25.5" spans="1:14">
       <c r="A21" s="6"/>
       <c r="B21" s="4" t="s">
         <v>70</v>
@@ -3807,36 +3931,36 @@
         <v>71</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="J21" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L21" s="17" t="s">
+      <c r="I21" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M21" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="N21" s="19"/>
+      <c r="M21" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="N21" s="18"/>
     </row>
-    <row r="22" ht="25.5" spans="1:14">
+    <row r="22" ht="63.75" spans="1:14">
       <c r="A22" s="6"/>
       <c r="B22" s="4" t="s">
         <v>70</v>
@@ -3845,100 +3969,102 @@
         <v>71</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L22" s="17" t="s">
+      <c r="H22" s="5">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="N22" s="19"/>
+      <c r="M22" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="N22" s="18"/>
     </row>
-    <row r="23" ht="63.75" spans="1:14">
+    <row r="23" spans="1:14">
       <c r="A23" s="6"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" ht="38.25" spans="1:14">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5">
-        <v>2000</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L23" s="17" t="s">
+      <c r="D24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="N23" s="19"/>
+      <c r="M24" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="N24" s="18"/>
     </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" ht="38.25" spans="1:14">
+    <row r="25" ht="51" spans="1:14">
       <c r="A25" s="6"/>
       <c r="B25" s="4" t="s">
         <v>70</v>
@@ -3947,34 +4073,34 @@
         <v>71</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="J25" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L25" s="17" t="s">
+      <c r="K25" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M25" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="N25" s="19"/>
+      <c r="M25" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="N25" s="18"/>
     </row>
     <row r="26" ht="51" spans="1:14">
       <c r="A26" s="6"/>
@@ -3985,34 +4111,34 @@
         <v>71</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" s="17" t="s">
+      <c r="H26" s="5">
+        <v>3395</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L26" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M26" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="N26" s="19"/>
+      <c r="M26" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="N26" s="18"/>
     </row>
     <row r="27" ht="51" spans="1:14">
       <c r="A27" s="6"/>
@@ -4023,36 +4149,36 @@
         <v>71</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="5">
-        <v>3395</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L27" s="17" t="s">
+      <c r="H27" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M27" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="N27" s="19"/>
+      <c r="M27" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="N27" s="18"/>
     </row>
-    <row r="28" ht="51" spans="1:14">
+    <row r="28" ht="25.5" spans="1:14">
       <c r="A28" s="6"/>
       <c r="B28" s="4" t="s">
         <v>70</v>
@@ -4061,34 +4187,34 @@
         <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L28" s="17" t="s">
+      <c r="H28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M28" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="N28" s="19"/>
+      <c r="M28" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="N28" s="18"/>
     </row>
     <row r="29" ht="25.5" spans="1:14">
       <c r="A29" s="6"/>
@@ -4099,34 +4225,34 @@
         <v>71</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L29" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="N29" s="19"/>
+      <c r="M29" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" ht="25.5" spans="1:14">
       <c r="A30" s="6"/>
@@ -4137,36 +4263,36 @@
         <v>71</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L30" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M30" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="N30" s="19"/>
+      <c r="M30" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="N30" s="18"/>
     </row>
-    <row r="31" ht="25.5" spans="1:14">
+    <row r="31" spans="1:14">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
         <v>70</v>
@@ -4175,34 +4301,34 @@
         <v>71</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="N31" s="19"/>
+        <v>32</v>
+      </c>
+      <c r="N31" s="18"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="6"/>
@@ -4213,36 +4339,36 @@
         <v>71</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J32" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="N32" s="19"/>
+      <c r="L32" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" customFormat="1" spans="1:14">
       <c r="A33" s="6"/>
       <c r="B33" s="4" t="s">
         <v>70</v>
@@ -4251,34 +4377,136 @@
         <v>71</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>11</v>
+        <v>165</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I33" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J33" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="N33" s="19"/>
+      <c r="L33" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="M33" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="N33" s="18"/>
+    </row>
+    <row r="34" customFormat="1" spans="1:14">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="M34" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="N34" s="18"/>
+    </row>
+    <row r="35" customFormat="1" spans="1:14">
+      <c r="A35" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="18"/>
+    </row>
+    <row r="36" customFormat="1" ht="140.25" spans="1:14">
+      <c r="A36" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated procedures - full reload data from Landing to Stg1, usp_write_event_log for logging procedures that were run
</commit_message>
<xml_diff>
--- a/mapping_docs/cars-com_card mapping.xlsx
+++ b/mapping_docs/cars-com_card mapping.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="177">
   <si>
     <t>Data Example lnd_cars-com_card</t>
   </si>
@@ -264,6 +264,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>GENERATE_UUID</t>
     </r>
     <r>
@@ -1114,19 +1121,10 @@
     <t>file:/C:/Users/gavri/PycharmProjects/car_ads_scrapper/scrapped_data/cars_com/json/2023-05-14-05-42-14/2021/price_50000-59999/https---www-cars-com-vehicledetail-58ea2312-4dac-416b-a479-7d068d02b03a-.json</t>
   </si>
   <si>
-    <t>dl_loaded_date</t>
-  </si>
-  <si>
-    <t>2023-04-20 10:21:56.576</t>
-  </si>
-  <si>
-    <t>2023-05-16 10:21:56.576</t>
-  </si>
-  <si>
     <t>CURRENT_TIMESTAMP</t>
   </si>
   <si>
-    <t>stg1_loaded_date</t>
+    <t>modified_date</t>
   </si>
   <si>
     <t>2023-04-29 01:19:40.000</t>
@@ -1186,9 +1184,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
@@ -1253,14 +1251,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1268,9 +1258,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1291,11 +1289,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1323,10 +1321,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1335,6 +1341,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1362,21 +1375,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1452,7 +1450,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1464,13 +1474,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1488,7 +1498,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1500,7 +1540,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1512,19 +1552,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1542,25 +1576,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1573,42 +1607,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1904,6 +1902,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1915,15 +1933,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1975,164 +1984,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2193,9 +2191,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2990,238 +2985,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:4">
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="15.75" spans="1:10">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="50" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="32">
         <v>212900</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="51" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>82996</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="28"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="34">
+      <c r="A6" s="33">
         <v>23070</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <v>29997</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="52" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>45669</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="52" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:10">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="38">
         <v>25795</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="53" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" ht="15.75"/>
     <row r="11" spans="1:4">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="45"/>
     </row>
     <row r="13" ht="15.75" spans="1:4">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="37" t="s">
+      <c r="B13" s="47"/>
+      <c r="C13" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="49"/>
+      <c r="D13" s="48"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="50"/>
+      <c r="B15" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3243,10 +3238,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N36"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4407,7 +4402,9 @@
       <c r="N33" s="18"/>
     </row>
     <row r="34" customFormat="1" spans="1:14">
-      <c r="A34" s="6"/>
+      <c r="A34" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="B34" s="4" t="s">
         <v>70</v>
       </c>
@@ -4415,7 +4412,7 @@
         <v>71</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>164</v>
@@ -4424,89 +4421,49 @@
         <v>74</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="M34" s="25" t="s">
+      <c r="H34" s="5" t="s">
         <v>169</v>
       </c>
+      <c r="I34" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="17"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" customFormat="1" spans="1:14">
-      <c r="A35" s="4" t="s">
-        <v>170</v>
+    <row r="35" customFormat="1" ht="140.25" spans="1:14">
+      <c r="A35" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="5" t="s">
-        <v>172</v>
+      <c r="H35" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="16"/>
-      <c r="M35" s="17"/>
+      <c r="M35" s="25"/>
       <c r="N35" s="18"/>
-    </row>
-    <row r="36" customFormat="1" ht="140.25" spans="1:14">
-      <c r="A36" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I36" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>